<commit_message>
Update Costs- Exception VarCost FT
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart2.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\Tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EDFD1D-D791-4380-8EB4-A0B8A20391FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2266D6FB-BE29-43D1-A0D4-D8984361B74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodity_labels" sheetId="1" r:id="rId1"/>
@@ -1997,10 +1997,10 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2049,12 +2049,12 @@
       <selection activeCell="A46" sqref="A28:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="26.59765625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="47.86328125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2580,11 +2580,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="42.73046875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
@@ -2622,9 +2622,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="32.140625" customWidth="1"/>
+    <col min="1" max="2" width="32.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2721,7 +2721,7 @@
       <selection activeCell="A2" sqref="A2:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="7" width="15" customWidth="1"/>
   </cols>
@@ -2760,9 +2760,9 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="6" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2798,12 +2798,12 @@
       <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="1" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="32.3984375" customWidth="1"/>
+    <col min="4" max="5" width="19.86328125" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2981,7 +2981,7 @@
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -3016,10 +3016,10 @@
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="1" max="4" width="13.73046875" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3052,10 +3052,10 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" customWidth="1"/>
+    <col min="3" max="3" width="43.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3280,16 +3280,16 @@
       <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
   <cols>
     <col min="1" max="1" width="10" style="4" customWidth="1"/>
     <col min="2" max="3" width="11" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="4" customWidth="1"/>
-    <col min="8" max="38" width="5.85546875" style="4" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="32.265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.86328125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" style="4" customWidth="1"/>
+    <col min="8" max="38" width="5.86328125" style="4" customWidth="1"/>
+    <col min="39" max="16384" width="9.1328125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="6" customFormat="1">
@@ -12403,14 +12403,14 @@
       <selection activeCell="A35" sqref="A7:A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="28.3984375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.265625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1">
@@ -12430,7 +12430,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
+    <row r="2" spans="1:5" ht="14.25">
       <c r="A2" t="s">
         <v>172</v>
       </c>
@@ -12444,7 +12444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5" ht="14.25">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -12462,7 +12462,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="14.25">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -12480,7 +12480,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" t="s">
         <v>178</v>
       </c>
@@ -12494,7 +12494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15">
+    <row r="6" spans="1:5" ht="14.25">
       <c r="A6" t="s">
         <v>179</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15">
+    <row r="7" spans="1:5" ht="14.25">
       <c r="A7" s="15" t="s">
         <v>180</v>
       </c>
@@ -12525,7 +12525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15">
+    <row r="8" spans="1:5" ht="14.25">
       <c r="A8" t="s">
         <v>181</v>
       </c>
@@ -12542,7 +12542,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15">
+    <row r="9" spans="1:5" ht="14.25">
       <c r="A9" t="s">
         <v>182</v>
       </c>
@@ -12560,7 +12560,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15">
+    <row r="10" spans="1:5" ht="14.25">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -12578,7 +12578,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15">
+    <row r="11" spans="1:5" ht="14.25">
       <c r="A11" t="s">
         <v>183</v>
       </c>
@@ -12596,7 +12596,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15">
+    <row r="12" spans="1:5" ht="14.25">
       <c r="A12" t="s">
         <v>183</v>
       </c>
@@ -12614,7 +12614,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15">
+    <row r="13" spans="1:5" ht="14.25">
       <c r="A13" t="s">
         <v>184</v>
       </c>
@@ -12631,7 +12631,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15">
+    <row r="14" spans="1:5" ht="14.25">
       <c r="A14" t="s">
         <v>186</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15">
+    <row r="15" spans="1:5" ht="14.25">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -12665,7 +12665,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15">
+    <row r="16" spans="1:5" ht="14.25">
       <c r="A16" t="s">
         <v>188</v>
       </c>
@@ -12682,7 +12682,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15">
+    <row r="17" spans="1:11" ht="14.25">
       <c r="A17" t="s">
         <v>194</v>
       </c>
@@ -12696,7 +12696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11" ht="14.25">
       <c r="A18" t="s">
         <v>195</v>
       </c>
@@ -12710,7 +12710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11" ht="14.25">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -12727,7 +12727,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15">
+    <row r="20" spans="1:11" ht="14.25">
       <c r="A20" t="s">
         <v>199</v>
       </c>
@@ -12745,7 +12745,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11" ht="14.25">
       <c r="A21" t="s">
         <v>199</v>
       </c>
@@ -12763,7 +12763,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15">
+    <row r="22" spans="1:11" ht="14.25">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -12781,7 +12781,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15">
+    <row r="23" spans="1:11" ht="14.25">
       <c r="A23" t="s">
         <v>200</v>
       </c>
@@ -12799,7 +12799,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15">
+    <row r="24" spans="1:11" ht="14.25">
       <c r="A24" t="s">
         <v>201</v>
       </c>
@@ -12816,7 +12816,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15">
+    <row r="25" spans="1:11" ht="14.25">
       <c r="A25" t="s">
         <v>202</v>
       </c>
@@ -12833,7 +12833,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15">
+    <row r="26" spans="1:11" ht="14.25">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -12851,7 +12851,7 @@
       </c>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="15">
+    <row r="27" spans="1:11" ht="14.25">
       <c r="A27" t="s">
         <v>204</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15">
+    <row r="28" spans="1:11" ht="14.25">
       <c r="A28" t="s">
         <v>204</v>
       </c>
@@ -12888,7 +12888,7 @@
       </c>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="15">
+    <row r="29" spans="1:11" ht="14.25">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -12906,7 +12906,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15">
+    <row r="30" spans="1:11" ht="14.25">
       <c r="A30" t="s">
         <v>205</v>
       </c>
@@ -12924,7 +12924,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15">
+    <row r="31" spans="1:11" ht="14.25">
       <c r="A31" t="s">
         <v>206</v>
       </c>
@@ -12941,7 +12941,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15">
+    <row r="32" spans="1:11" ht="14.25">
       <c r="A32" t="s">
         <v>207</v>
       </c>
@@ -12958,7 +12958,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15">
+    <row r="33" spans="1:4" ht="14.25">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -12972,7 +12972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15">
+    <row r="34" spans="1:4" ht="14.25">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -12986,7 +12986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15">
+    <row r="35" spans="1:4" ht="14.25">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -13129,16 +13129,16 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1328125" style="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="19.5703125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="27.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="8" width="9.1328125" style="1"/>
+    <col min="9" max="9" width="19.59765625" style="1" customWidth="1"/>
+    <col min="10" max="12" width="27.1328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.59765625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="9:10">
@@ -13458,13 +13458,13 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="4" width="12.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="76.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.1328125" customWidth="1"/>
+    <col min="2" max="4" width="12.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="76.59765625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1">
@@ -13741,15 +13741,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="4" customWidth="1"/>
+    <col min="1" max="2" width="11.3984375" style="4" customWidth="1"/>
     <col min="3" max="3" width="10" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="4" customWidth="1"/>
-    <col min="7" max="38" width="6.140625" style="4" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="21.265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.1328125" style="4" customWidth="1"/>
+    <col min="7" max="38" width="6.1328125" style="4" customWidth="1"/>
+    <col min="39" max="16384" width="9.1328125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -16027,13 +16027,13 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="65.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="21.265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="1"/>
+    <col min="4" max="4" width="65.59765625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
@@ -16158,14 +16158,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="8" customWidth="1"/>
-    <col min="4" max="34" width="6.85546875" style="8" customWidth="1"/>
-    <col min="35" max="39" width="7.42578125" style="8" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.265625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="29.86328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" style="8" customWidth="1"/>
+    <col min="4" max="34" width="6.86328125" style="8" customWidth="1"/>
+    <col min="35" max="39" width="7.3984375" style="8" customWidth="1"/>
+    <col min="40" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="3" customFormat="1">

</xml_diff>

<commit_message>
Improve transmission and interchange
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart2.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09BEFC7-5321-4B87-A7A4-539062188E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B53CBF-4F92-4C77-8AED-E840465149F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="849" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodity_labels" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <sheet name="MaxActivity" sheetId="20" r:id="rId16"/>
     <sheet name="MinActivity" sheetId="19" r:id="rId17"/>
     <sheet name="MaxResource" sheetId="16" r:id="rId18"/>
-    <sheet name="Sheet1" sheetId="22" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6851" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6928" uniqueCount="363">
   <si>
     <t>p</t>
   </si>
@@ -956,19 +955,10 @@
     <t>GENERAL_CO2_CAP</t>
   </si>
   <si>
-    <t>ENERGY_INTERCHANGE</t>
-  </si>
-  <si>
-    <t>Interchange of Energy in/out of NC</t>
-  </si>
-  <si>
     <t>Tech Used to Represent Other Options For CO2 Capture</t>
   </si>
   <si>
     <t>Convert At CO2 to Captured CO2</t>
-  </si>
-  <si>
-    <t>Need to model this. What is the emission on imports</t>
   </si>
   <si>
     <t>ATB 2022 C6 Tech</t>
@@ -1122,6 +1112,42 @@
   </si>
   <si>
     <t>PJ/PJ</t>
+  </si>
+  <si>
+    <t>Assume Capacity Credit of NG Plants (Enforced on Contracts)</t>
+  </si>
+  <si>
+    <t>10.25% of Demand from EIA NC Summary Statistics</t>
+  </si>
+  <si>
+    <t>Determined from Simulation of the Model (&lt;2023)</t>
+  </si>
+  <si>
+    <t>Max growth of 0.82% Year (Terminal load growth) from 2023</t>
+  </si>
+  <si>
+    <t>Losses are accounted later on Transmission Regional</t>
+  </si>
+  <si>
+    <t>dummy- This tech has no capital cost</t>
+  </si>
+  <si>
+    <t>Emissions here are based on forecasts from EIA-AEO23, these emissions are assigned using the python code and import Excel 1 table as they are period dependent</t>
+  </si>
+  <si>
+    <t>ENERGY_IMPORT_S1</t>
+  </si>
+  <si>
+    <t>ENERGY_IMPORT_S2</t>
+  </si>
+  <si>
+    <t>ELC_IMP</t>
+  </si>
+  <si>
+    <t>Intermediary imput for the energy import (Used to help account for emissions changing with the period)</t>
+  </si>
+  <si>
+    <t>10.25% of Demand from EIA NC Summary Statistics - At Least 50% of this value</t>
   </si>
 </sst>
 </file>
@@ -3094,10 +3120,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7BDD85-BE5C-43DC-B5E7-A7EA8EDFC2F3}">
-  <dimension ref="A1:AH51"/>
+  <dimension ref="A1:AH52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:B51"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
@@ -6854,12 +6880,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:34">
+    <row r="37" spans="1:34" ht="15">
       <c r="A37" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="21" t="s">
-        <v>298</v>
+      <c r="B37" s="39" t="s">
+        <v>344</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>128</v>
@@ -6963,7 +6989,7 @@
         <v>6</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>128</v>
@@ -7067,7 +7093,7 @@
         <v>6</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>128</v>
@@ -7171,7 +7197,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>128</v>
@@ -7275,7 +7301,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>128</v>
@@ -7379,7 +7405,7 @@
         <v>6</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>128</v>
@@ -7483,7 +7509,7 @@
         <v>6</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>128</v>
@@ -7586,104 +7612,104 @@
       <c r="A44" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>128</v>
-      </c>
       <c r="D44" s="6">
-        <v>0.05</v>
+        <v>6.5421499999999994E-2</v>
       </c>
       <c r="E44" s="6">
-        <v>0.05</v>
+        <v>6.5421499999999994E-2</v>
       </c>
       <c r="F44" s="6">
-        <v>0.05</v>
+        <v>6.5421499999999994E-2</v>
       </c>
       <c r="G44" s="6">
-        <v>0.05</v>
+        <v>6.5421499999999994E-2</v>
       </c>
       <c r="H44" s="6">
-        <v>0.05</v>
+        <v>6.5421499999999994E-2</v>
       </c>
       <c r="I44" s="6">
-        <v>0.05</v>
+        <v>6.5421499999999994E-2</v>
       </c>
       <c r="J44" s="6">
-        <v>0.05</v>
+        <v>6.3967868046929291E-2</v>
       </c>
       <c r="K44" s="6">
-        <v>0.05</v>
+        <v>6.2624104812130876E-2</v>
       </c>
       <c r="L44" s="6">
-        <v>0.05</v>
+        <v>6.1390210295604764E-2</v>
       </c>
       <c r="M44" s="6">
-        <v>0.05</v>
+        <v>6.0266184497350932E-2</v>
       </c>
       <c r="N44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="O44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="P44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="Q44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="R44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="S44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="T44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="U44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="V44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="W44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="X44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="Y44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="Z44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AA44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AB44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AC44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AD44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AE44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AF44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AG44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
       <c r="AH44" s="6">
-        <v>0.05</v>
+        <v>5.9252027417369402E-2</v>
       </c>
     </row>
     <row r="45" spans="1:34" ht="15">
@@ -7691,10 +7717,10 @@
         <v>6</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D45" s="6">
         <v>6.5421499999999994E-2</v>
@@ -7795,10 +7821,10 @@
         <v>6</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>351</v>
+        <v>311</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D46" s="6">
         <v>6.5421499999999994E-2</v>
@@ -7899,10 +7925,10 @@
         <v>6</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D47" s="6">
         <v>6.5421499999999994E-2</v>
@@ -8003,10 +8029,10 @@
         <v>6</v>
       </c>
       <c r="B48" s="34" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D48" s="6">
         <v>6.5421499999999994E-2</v>
@@ -8107,10 +8133,10 @@
         <v>6</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>316</v>
+        <v>349</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D49" s="6">
         <v>6.5421499999999994E-2</v>
@@ -8128,19 +8154,19 @@
         <v>6.5421499999999994E-2</v>
       </c>
       <c r="I49" s="6">
-        <v>6.5421499999999994E-2</v>
+        <v>6.3483644739827622E-2</v>
       </c>
       <c r="J49" s="6">
-        <v>6.3967868046929291E-2</v>
+        <v>6.2454206744882147E-2</v>
       </c>
       <c r="K49" s="6">
-        <v>6.2624104812130876E-2</v>
+        <v>6.1516326015163603E-2</v>
       </c>
       <c r="L49" s="6">
-        <v>6.1390210295604764E-2</v>
+        <v>6.0670002550671967E-2</v>
       </c>
       <c r="M49" s="6">
-        <v>6.0266184497350932E-2</v>
+        <v>5.9915236351407233E-2</v>
       </c>
       <c r="N49" s="6">
         <v>5.9252027417369402E-2</v>
@@ -8211,10 +8237,10 @@
         <v>6</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D50" s="6">
         <v>6.5421499999999994E-2</v>
@@ -8310,108 +8336,212 @@
         <v>5.9252027417369402E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:34" ht="15">
+    <row r="51" spans="1:34">
       <c r="A51" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="34" t="s">
-        <v>317</v>
+      <c r="B51" s="6" t="s">
+        <v>358</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="D51" s="6">
-        <v>6.5421499999999994E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E51" s="6">
-        <v>6.5421499999999994E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F51" s="6">
-        <v>6.5421499999999994E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G51" s="6">
-        <v>6.5421499999999994E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H51" s="6">
-        <v>6.5421499999999994E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I51" s="6">
-        <v>6.3483644739827622E-2</v>
+        <v>0.05</v>
       </c>
       <c r="J51" s="6">
-        <v>6.2454206744882147E-2</v>
+        <v>0.05</v>
       </c>
       <c r="K51" s="6">
-        <v>6.1516326015163603E-2</v>
+        <v>0.05</v>
       </c>
       <c r="L51" s="6">
-        <v>6.0670002550671967E-2</v>
+        <v>0.05</v>
       </c>
       <c r="M51" s="6">
-        <v>5.9915236351407233E-2</v>
+        <v>0.05</v>
       </c>
       <c r="N51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="O51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="P51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="Q51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="S51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="T51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="U51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="V51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="W51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="X51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="Y51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="Z51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AA51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AB51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AC51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AD51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AE51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AF51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AG51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AH51" s="6">
-        <v>5.9252027417369402E-2</v>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34">
+      <c r="A52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="E52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="F52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="H52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="I52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="J52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="K52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="L52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="M52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="N52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="O52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="P52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="R52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="S52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="T52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="U52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="V52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="W52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="X52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="Y52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="Z52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AA52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AB52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AC52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AD52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AE52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AF52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AG52" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AH52" s="6">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -8425,10 +8555,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41267312-A157-4F65-86B7-C35DBAD3B2EE}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
@@ -8932,6 +9062,28 @@
       </c>
       <c r="C45" s="6" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -9088,8 +9240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA9BB2C-9F9E-4D6B-AAF2-83D7B122A42E}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD185"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9255,7 +9407,7 @@
         <v>282</v>
       </c>
       <c r="F9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -9275,7 +9427,7 @@
         <v>282</v>
       </c>
       <c r="F10" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -9295,7 +9447,7 @@
         <v>282</v>
       </c>
       <c r="F11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -9315,7 +9467,7 @@
         <v>282</v>
       </c>
       <c r="F12" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -9335,7 +9487,7 @@
         <v>282</v>
       </c>
       <c r="F13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -9355,7 +9507,7 @@
         <v>282</v>
       </c>
       <c r="F14" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -9375,7 +9527,7 @@
         <v>282</v>
       </c>
       <c r="F15" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -9395,7 +9547,7 @@
         <v>282</v>
       </c>
       <c r="F16" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -9415,7 +9567,7 @@
         <v>282</v>
       </c>
       <c r="F17" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -9435,7 +9587,7 @@
         <v>282</v>
       </c>
       <c r="F18" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -9455,7 +9607,7 @@
         <v>282</v>
       </c>
       <c r="F19" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -9475,7 +9627,7 @@
         <v>282</v>
       </c>
       <c r="F20" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -9495,7 +9647,7 @@
         <v>282</v>
       </c>
       <c r="F21" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -9515,7 +9667,7 @@
         <v>282</v>
       </c>
       <c r="F22" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -9535,7 +9687,7 @@
         <v>282</v>
       </c>
       <c r="F23" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -9555,7 +9707,7 @@
         <v>282</v>
       </c>
       <c r="F24" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -9575,7 +9727,7 @@
         <v>282</v>
       </c>
       <c r="F25" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -9595,7 +9747,7 @@
         <v>282</v>
       </c>
       <c r="F26" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -9615,7 +9767,7 @@
         <v>282</v>
       </c>
       <c r="F27" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -9635,7 +9787,7 @@
         <v>282</v>
       </c>
       <c r="F28" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -9655,7 +9807,7 @@
         <v>282</v>
       </c>
       <c r="F29" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -9666,7 +9818,7 @@
         <v>2023</v>
       </c>
       <c r="C30" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -9675,7 +9827,7 @@
         <v>282</v>
       </c>
       <c r="F30" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -9686,16 +9838,17 @@
         <v>2025</v>
       </c>
       <c r="C31" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D31">
+        <f>D30*1.0082^(B31-B30)</f>
         <v>0</v>
       </c>
       <c r="E31" t="s">
         <v>282</v>
       </c>
       <c r="F31" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -9706,16 +9859,17 @@
         <v>2030</v>
       </c>
       <c r="C32" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D32">
+        <f t="shared" ref="D32:D36" si="0">D31*1.0082^(B32-B31)</f>
         <v>0</v>
       </c>
       <c r="E32" t="s">
         <v>282</v>
       </c>
       <c r="F32" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -9726,16 +9880,17 @@
         <v>2035</v>
       </c>
       <c r="C33" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D33">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E33" t="s">
         <v>282</v>
       </c>
       <c r="F33" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -9746,16 +9901,17 @@
         <v>2040</v>
       </c>
       <c r="C34" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D34">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E34" t="s">
         <v>282</v>
       </c>
       <c r="F34" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -9766,16 +9922,17 @@
         <v>2045</v>
       </c>
       <c r="C35" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D35">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E35" t="s">
         <v>282</v>
       </c>
       <c r="F35" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -9786,16 +9943,17 @@
         <v>2050</v>
       </c>
       <c r="C36" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D36">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E36" t="s">
         <v>282</v>
       </c>
       <c r="F36" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -9806,16 +9964,16 @@
         <v>2023</v>
       </c>
       <c r="C37" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1.83</v>
       </c>
       <c r="E37" t="s">
         <v>282</v>
       </c>
       <c r="F37" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -9826,16 +9984,17 @@
         <v>2025</v>
       </c>
       <c r="C38" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <f>D37*1.0082^(B38-B37)</f>
+        <v>1.8601350491999999</v>
       </c>
       <c r="E38" t="s">
         <v>282</v>
       </c>
       <c r="F38" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -9846,16 +10005,17 @@
         <v>2030</v>
       </c>
       <c r="C39" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <f t="shared" ref="D39:D43" si="1">D38*1.0082^(B39-B38)</f>
+        <v>1.937661639333039</v>
       </c>
       <c r="E39" t="s">
         <v>282</v>
       </c>
       <c r="F39" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -9866,16 +10026,17 @@
         <v>2035</v>
       </c>
       <c r="C40" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.0184193777529948</v>
       </c>
       <c r="E40" t="s">
         <v>282</v>
       </c>
       <c r="F40" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -9886,16 +10047,17 @@
         <v>2040</v>
       </c>
       <c r="C41" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1025429320524203</v>
       </c>
       <c r="E41" t="s">
         <v>282</v>
       </c>
       <c r="F41" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -9906,16 +10068,17 @@
         <v>2045</v>
       </c>
       <c r="C42" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.1901725824912153</v>
       </c>
       <c r="E42" t="s">
         <v>282</v>
       </c>
       <c r="F42" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -9926,16 +10089,17 @@
         <v>2050</v>
       </c>
       <c r="C43" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.2814544559210193</v>
       </c>
       <c r="E43" t="s">
         <v>282</v>
       </c>
       <c r="F43" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -9946,16 +10110,16 @@
         <v>2023</v>
       </c>
       <c r="C44" t="s">
-        <v>298</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
+        <v>358</v>
+      </c>
+      <c r="D44" s="1">
+        <v>4.6760999999999999</v>
       </c>
       <c r="E44" t="s">
         <v>282</v>
       </c>
       <c r="F44" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -9966,16 +10130,17 @@
         <v>2025</v>
       </c>
       <c r="C45" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <f>D44*1.0082^(B45-B44)</f>
+        <v>4.7531024609639996</v>
       </c>
       <c r="E45" t="s">
         <v>282</v>
       </c>
       <c r="F45" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -9986,16 +10151,17 @@
         <v>2030</v>
       </c>
       <c r="C46" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <f>D45*1.0082^(B46-B45)</f>
+        <v>4.9512019626695212</v>
       </c>
       <c r="E46" t="s">
         <v>282</v>
       </c>
       <c r="F46" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -10006,16 +10172,17 @@
         <v>2035</v>
       </c>
       <c r="C47" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <f t="shared" ref="D47:D50" si="2">D46*1.0082^(B47-B46)</f>
+        <v>5.1575578427927757</v>
       </c>
       <c r="E47" t="s">
         <v>282</v>
       </c>
       <c r="F47" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -10026,16 +10193,17 @@
         <v>2040</v>
       </c>
       <c r="C48" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.3725142101477168</v>
       </c>
       <c r="E48" t="s">
         <v>282</v>
       </c>
       <c r="F48" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -10046,16 +10214,17 @@
         <v>2045</v>
       </c>
       <c r="C49" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.5964295152935355</v>
       </c>
       <c r="E49" t="s">
         <v>282</v>
       </c>
       <c r="F49" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -10066,16 +10235,17 @@
         <v>2050</v>
       </c>
       <c r="C50" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5.8296771482690026</v>
       </c>
       <c r="E50" t="s">
         <v>282</v>
       </c>
       <c r="F50" t="s">
-        <v>308</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -10090,7 +10260,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10125,10 +10295,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C981D50-80F8-4166-95FD-5AC25F26EC3C}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="A9" sqref="A9:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10299,6 +10469,153 @@
         <v>126</v>
       </c>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9">
+        <v>2023</v>
+      </c>
+      <c r="C9" t="s">
+        <v>358</v>
+      </c>
+      <c r="D9">
+        <f>521.092380734395*0.125</f>
+        <v>65.136547591799371</v>
+      </c>
+      <c r="E9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10">
+        <v>2025</v>
+      </c>
+      <c r="C10" t="s">
+        <v>358</v>
+      </c>
+      <c r="D10">
+        <f>0.125*523.765108258534</f>
+        <v>65.470638532316755</v>
+      </c>
+      <c r="E10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11">
+        <v>2030</v>
+      </c>
+      <c r="C11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11">
+        <f>0.125*538.34157772492</f>
+        <v>67.292697215614993</v>
+      </c>
+      <c r="E11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12">
+        <v>2035</v>
+      </c>
+      <c r="C12" t="s">
+        <v>358</v>
+      </c>
+      <c r="D12">
+        <f>0.125*567.850454710087</f>
+        <v>70.981306838760872</v>
+      </c>
+      <c r="E12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13">
+        <v>2040</v>
+      </c>
+      <c r="C13" t="s">
+        <v>358</v>
+      </c>
+      <c r="D13">
+        <f>0.125*597.03498893503</f>
+        <v>74.629373616878752</v>
+      </c>
+      <c r="E13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14">
+        <v>2045</v>
+      </c>
+      <c r="C14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14">
+        <f>0.125*624.264150183609</f>
+        <v>78.033018772951124</v>
+      </c>
+      <c r="E14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15">
+        <v>2050</v>
+      </c>
+      <c r="C15" t="s">
+        <v>358</v>
+      </c>
+      <c r="D15">
+        <f>0.125*653.043332059524</f>
+        <v>81.630416507440501</v>
+      </c>
+      <c r="E15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" t="s">
+        <v>352</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10308,10 +10625,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DEEE4BE-FD88-49A2-A041-525121977217}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10869,7 +11186,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>277</v>
       </c>
@@ -10886,7 +11203,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>277</v>
       </c>
@@ -10903,7 +11220,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>277</v>
       </c>
@@ -10920,7 +11237,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>277</v>
       </c>
@@ -10937,7 +11254,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>278</v>
       </c>
@@ -10954,7 +11271,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>278</v>
       </c>
@@ -10971,7 +11288,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>278</v>
       </c>
@@ -10988,7 +11305,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>278</v>
       </c>
@@ -11005,7 +11322,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>278</v>
       </c>
@@ -11022,7 +11339,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>278</v>
       </c>
@@ -11039,7 +11356,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>278</v>
       </c>
@@ -11054,6 +11371,153 @@
       </c>
       <c r="E43" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44">
+        <v>2023</v>
+      </c>
+      <c r="C44" t="s">
+        <v>358</v>
+      </c>
+      <c r="D44">
+        <f>521.092380734395*0.125</f>
+        <v>65.136547591799371</v>
+      </c>
+      <c r="E44" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45">
+        <v>2025</v>
+      </c>
+      <c r="C45" t="s">
+        <v>358</v>
+      </c>
+      <c r="D45">
+        <f>0.125*523.765108258534*0.98</f>
+        <v>64.161225761670423</v>
+      </c>
+      <c r="E45" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46">
+        <v>2030</v>
+      </c>
+      <c r="C46" t="s">
+        <v>358</v>
+      </c>
+      <c r="D46">
+        <f>0.125*538.34157772492*0.93</f>
+        <v>62.58220841052195</v>
+      </c>
+      <c r="E46" t="s">
+        <v>125</v>
+      </c>
+      <c r="F46" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47">
+        <v>2035</v>
+      </c>
+      <c r="C47" t="s">
+        <v>358</v>
+      </c>
+      <c r="D47">
+        <f>0.125*567.850454710087*0.88</f>
+        <v>62.463550018109565</v>
+      </c>
+      <c r="E47" t="s">
+        <v>125</v>
+      </c>
+      <c r="F47" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48">
+        <v>2040</v>
+      </c>
+      <c r="C48" t="s">
+        <v>358</v>
+      </c>
+      <c r="D48">
+        <f>0.125*597.03498893503*0.83</f>
+        <v>61.942380102009359</v>
+      </c>
+      <c r="E48" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49">
+        <v>2045</v>
+      </c>
+      <c r="C49" t="s">
+        <v>358</v>
+      </c>
+      <c r="D49">
+        <f>0.125*624.264150183609*0.78</f>
+        <v>60.865754642901877</v>
+      </c>
+      <c r="E49" t="s">
+        <v>125</v>
+      </c>
+      <c r="F49" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B50">
+        <v>2050</v>
+      </c>
+      <c r="C50" t="s">
+        <v>358</v>
+      </c>
+      <c r="D50">
+        <f>0.125*653.043332059524*0.73</f>
+        <v>59.590204050431566</v>
+      </c>
+      <c r="E50" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -11066,7 +11530,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="B22:E37"/>
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11097,24 +11561,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E06B6E-6CDB-4D8C-BC34-6B8026E57C73}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F345D6D4-C1C5-41B3-9FA9-983E075A149F}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11169,13 +11621,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -11312,13 +11764,13 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -11345,90 +11797,101 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>332</v>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>360</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -11438,10 +11901,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B94D054-32A6-4BDE-98D7-472A0F6D7282}">
-  <dimension ref="A1:AL105"/>
+  <dimension ref="A1:AL104"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="E58:G60"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
@@ -11708,7 +12171,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H3" s="35">
         <v>9.6251902779803084E-2</v>
@@ -12746,7 +13209,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H12" s="43">
         <v>0.12549199999999999</v>
@@ -12862,7 +13325,7 @@
         <v>19</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H13" s="43">
         <v>8.6045161319189351E-2</v>
@@ -13797,7 +14260,7 @@
         <v>204</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>14</v>
@@ -15437,7 +15900,7 @@
         <v>16</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H35" s="35">
         <v>0.11778563015312131</v>
@@ -15553,7 +16016,7 @@
         <v>16</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H36" s="35">
         <v>0.11778563015312131</v>
@@ -15669,7 +16132,7 @@
         <v>16</v>
       </c>
       <c r="G37" s="35" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H37" s="35">
         <v>0.11778563015312131</v>
@@ -15773,7 +16236,7 @@
         <v>6</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E38" s="21" t="s">
         <v>296</v>
@@ -16704,7 +17167,7 @@
         <v>19</v>
       </c>
       <c r="G46" s="42" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H46" s="4">
         <v>0.15723270440251572</v>
@@ -16820,7 +17283,7 @@
         <v>19</v>
       </c>
       <c r="G47" s="42" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H47" s="4">
         <v>0.15723270440251572</v>
@@ -16936,7 +17399,7 @@
         <v>19</v>
       </c>
       <c r="G48" s="42" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H48" s="4">
         <v>0.15723270440251572</v>
@@ -17052,7 +17515,7 @@
         <v>19</v>
       </c>
       <c r="G49" s="42" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H49" s="4">
         <v>0.10288065843621398</v>
@@ -17168,7 +17631,7 @@
         <v>19</v>
       </c>
       <c r="G50" s="42" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H50" s="4">
         <v>0.10288065843621398</v>
@@ -17284,7 +17747,7 @@
         <v>19</v>
       </c>
       <c r="G51" s="42" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H51" s="4">
         <v>0.10288065843621398</v>
@@ -18096,7 +18559,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="42" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H58" s="4">
         <v>0.16129032258064516</v>
@@ -18212,7 +18675,7 @@
         <v>19</v>
       </c>
       <c r="G59" s="42" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H59" s="4">
         <v>0.16129032258064516</v>
@@ -18328,7 +18791,7 @@
         <v>19</v>
       </c>
       <c r="G60" s="42" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="H60" s="4">
         <v>0.16129032258064516</v>
@@ -18827,7 +19290,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="E64" s="21" t="s">
         <v>295</v>
@@ -19509,7 +19972,7 @@
         <v>149</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>147</v>
@@ -19623,7 +20086,7 @@
         <v>172</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>16</v>
@@ -19736,7 +20199,7 @@
         <v>144</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>19</v>
@@ -19849,7 +20312,7 @@
         <v>173</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>21</v>
@@ -19962,7 +20425,7 @@
         <v>174</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>25</v>
@@ -20553,16 +21016,16 @@
       </c>
       <c r="C79" s="23"/>
       <c r="D79" s="21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E79" s="21" t="s">
         <v>297</v>
       </c>
       <c r="F79" s="38" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G79" s="38" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H79" s="22">
         <v>1</v>
@@ -20658,117 +21121,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:38" s="24" customFormat="1">
+    <row r="80" spans="1:38">
       <c r="A80" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B80" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="23"/>
-      <c r="D80" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="E80" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="F80" s="23" t="s">
-        <v>333</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H80" s="22">
-        <v>1</v>
-      </c>
-      <c r="I80" s="22">
-        <v>1</v>
-      </c>
-      <c r="J80" s="22">
-        <v>1</v>
-      </c>
-      <c r="K80" s="22">
-        <v>1</v>
-      </c>
-      <c r="L80" s="22">
-        <v>1</v>
-      </c>
-      <c r="M80" s="22">
-        <v>1</v>
-      </c>
-      <c r="N80" s="22">
-        <v>1</v>
-      </c>
-      <c r="O80" s="22">
-        <v>1</v>
-      </c>
-      <c r="P80" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q80" s="22">
-        <v>1</v>
-      </c>
-      <c r="R80" s="22">
-        <v>1</v>
-      </c>
-      <c r="S80" s="22">
-        <v>1</v>
-      </c>
-      <c r="T80" s="22">
-        <v>1</v>
-      </c>
-      <c r="U80" s="22">
-        <v>1</v>
-      </c>
-      <c r="V80" s="22">
-        <v>1</v>
-      </c>
-      <c r="W80" s="22">
-        <v>1</v>
-      </c>
-      <c r="X80" s="22">
-        <v>1</v>
-      </c>
-      <c r="Y80" s="22">
-        <v>1</v>
-      </c>
-      <c r="Z80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AA80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AB80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AC80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AD80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AE80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AF80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AG80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AH80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AI80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AJ80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AK80" s="22">
-        <v>1</v>
-      </c>
-      <c r="AL80" s="22">
+      <c r="C80" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E80" s="40" t="s">
+        <v>344</v>
+      </c>
+      <c r="F80" s="42" t="s">
+        <v>317</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="4">
+        <v>1</v>
+      </c>
+      <c r="I80" s="4">
+        <v>1</v>
+      </c>
+      <c r="J80" s="4">
+        <v>1</v>
+      </c>
+      <c r="K80" s="4">
+        <v>1</v>
+      </c>
+      <c r="L80" s="4">
+        <v>1</v>
+      </c>
+      <c r="M80" s="4">
+        <v>1</v>
+      </c>
+      <c r="N80" s="4">
+        <v>1</v>
+      </c>
+      <c r="O80" s="4">
+        <v>1</v>
+      </c>
+      <c r="P80" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="4">
+        <v>1</v>
+      </c>
+      <c r="R80" s="4">
+        <v>1</v>
+      </c>
+      <c r="S80" s="4">
+        <v>1</v>
+      </c>
+      <c r="T80" s="4">
+        <v>1</v>
+      </c>
+      <c r="U80" s="4">
+        <v>1</v>
+      </c>
+      <c r="V80" s="4">
+        <v>1</v>
+      </c>
+      <c r="W80" s="4">
+        <v>1</v>
+      </c>
+      <c r="X80" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y80" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK80" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL80" s="4">
         <v>1</v>
       </c>
     </row>
@@ -20780,16 +21245,16 @@
         <v>6</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E81" s="40" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F81" s="42" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>14</v>
@@ -20896,16 +21361,16 @@
         <v>6</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E82" s="40" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="F82" s="42" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>14</v>
@@ -21012,16 +21477,16 @@
         <v>6</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E83" s="40" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F83" s="42" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>14</v>
@@ -21128,16 +21593,16 @@
         <v>6</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E84" s="40" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F84" s="42" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>14</v>
@@ -21244,16 +21709,16 @@
         <v>6</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E85" s="40" t="s">
-        <v>337</v>
-      </c>
-      <c r="F85" s="42" t="s">
-        <v>327</v>
+        <v>346</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>310</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>14</v>
@@ -21360,16 +21825,16 @@
         <v>6</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E86" s="40" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>14</v>
@@ -21476,112 +21941,112 @@
         <v>6</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="E87" s="40" t="s">
-        <v>338</v>
+        <v>337</v>
+      </c>
+      <c r="E87" s="41" t="s">
+        <v>347</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="L87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="M87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="O87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="P87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="Q87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="R87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="S87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="T87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="U87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="V87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="W87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="X87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="Y87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="Z87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AA87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AB87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AC87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AD87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AE87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AF87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AG87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AH87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AI87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AJ87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AK87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AL87" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="88" spans="1:38">
@@ -21592,16 +22057,16 @@
         <v>6</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E88" s="41" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>14</v>
@@ -21708,16 +22173,16 @@
         <v>6</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E89" s="41" t="s">
-        <v>351</v>
+        <v>311</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>14</v>
@@ -21824,16 +22289,16 @@
         <v>6</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E90" s="41" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>14</v>
@@ -21940,16 +22405,16 @@
         <v>6</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E91" s="41" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>14</v>
@@ -22056,112 +22521,112 @@
         <v>6</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E92" s="41" t="s">
-        <v>316</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>327</v>
+        <v>349</v>
+      </c>
+      <c r="F92" s="42" t="s">
+        <v>310</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="I92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="K92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="L92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="M92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="N92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="P92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="Q92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="R92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="S92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="T92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="U92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="V92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="W92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="X92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="Y92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="Z92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AA92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AB92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AC92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AD92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AE92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AF92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AG92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AH92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AI92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AJ92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AK92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AL92" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="93" spans="1:38">
@@ -22172,16 +22637,16 @@
         <v>6</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E93" s="41" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="F93" s="42" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>14</v>
@@ -22281,120 +22746,233 @@
       </c>
     </row>
     <row r="94" spans="1:38">
-      <c r="A94" s="22" t="s">
+      <c r="A94" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B94" s="23" t="s">
+      <c r="B94" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>353</v>
-      </c>
       <c r="D94" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="E94" s="41" t="s">
-        <v>317</v>
-      </c>
-      <c r="F94" s="42" t="s">
-        <v>318</v>
+        <v>355</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>330</v>
       </c>
       <c r="G94" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="H94" s="4">
+        <v>1</v>
+      </c>
+      <c r="I94" s="4">
+        <v>1</v>
+      </c>
+      <c r="J94" s="4">
+        <v>1</v>
+      </c>
+      <c r="K94" s="4">
+        <v>1</v>
+      </c>
+      <c r="L94" s="4">
+        <v>1</v>
+      </c>
+      <c r="M94" s="4">
+        <v>1</v>
+      </c>
+      <c r="N94" s="4">
+        <v>1</v>
+      </c>
+      <c r="O94" s="4">
+        <v>1</v>
+      </c>
+      <c r="P94" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q94" s="4">
+        <v>1</v>
+      </c>
+      <c r="R94" s="4">
+        <v>1</v>
+      </c>
+      <c r="S94" s="4">
+        <v>1</v>
+      </c>
+      <c r="T94" s="4">
+        <v>1</v>
+      </c>
+      <c r="U94" s="4">
+        <v>1</v>
+      </c>
+      <c r="V94" s="4">
+        <v>1</v>
+      </c>
+      <c r="W94" s="4">
+        <v>1</v>
+      </c>
+      <c r="X94" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y94" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK94" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL94" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:38">
+      <c r="A95" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="G95" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="I94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="J94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="K94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="L94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="M94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="N94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="O94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="P94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="Q94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="R94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="S94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="T94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="U94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="V94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="W94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="X94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="Y94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="Z94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AA94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AB94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AC94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AD94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AE94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AF94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AG94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AH94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AI94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AJ94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AK94" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="AL94" s="4">
-        <v>0.7</v>
-      </c>
+      <c r="H95" s="4">
+        <v>1</v>
+      </c>
+      <c r="I95" s="4">
+        <v>1</v>
+      </c>
+      <c r="J95" s="4">
+        <v>1</v>
+      </c>
+      <c r="K95" s="4">
+        <v>1</v>
+      </c>
+      <c r="L95" s="4">
+        <v>1</v>
+      </c>
+      <c r="M95" s="4">
+        <v>1</v>
+      </c>
+      <c r="N95" s="4">
+        <v>1</v>
+      </c>
+      <c r="O95" s="4">
+        <v>1</v>
+      </c>
+      <c r="P95" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q95" s="4">
+        <v>1</v>
+      </c>
+      <c r="R95" s="4">
+        <v>1</v>
+      </c>
+      <c r="S95" s="4">
+        <v>1</v>
+      </c>
+      <c r="T95" s="4">
+        <v>1</v>
+      </c>
+      <c r="U95" s="4">
+        <v>1</v>
+      </c>
+      <c r="V95" s="4">
+        <v>1</v>
+      </c>
+      <c r="W95" s="4">
+        <v>1</v>
+      </c>
+      <c r="X95" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y95" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AI95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AJ95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK95" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL95" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" ht="15">
+      <c r="D98"/>
     </row>
     <row r="99" spans="4:4" ht="15">
       <c r="D99"/>
@@ -22413,9 +22991,6 @@
     </row>
     <row r="104" spans="4:4" ht="15">
       <c r="D104"/>
-    </row>
-    <row r="105" spans="4:4" ht="15">
-      <c r="D105"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -22426,10 +23001,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8BE285-5D8E-4DFA-BA36-7C02503E1408}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -22456,7 +23031,7 @@
         <v>64</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>65</v>
@@ -22476,7 +23051,7 @@
         <v>66</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E2" s="32">
         <v>0</v>
@@ -22488,13 +23063,13 @@
         <v>162</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E3" s="44">
         <f>214.126547670066</f>
@@ -22515,7 +23090,7 @@
         <v>66</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E4" s="32">
         <v>0</v>
@@ -22533,7 +23108,7 @@
         <v>66</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E5" s="32">
         <v>229.79396321542464</v>
@@ -22553,7 +23128,7 @@
         <v>66</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E6" s="32">
         <v>229.79396321542464</v>
@@ -22573,7 +23148,7 @@
         <v>66</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E7" s="32">
         <v>229.79396321542464</v>
@@ -22593,7 +23168,7 @@
         <v>66</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E8" s="32">
         <v>0</v>
@@ -22611,7 +23186,7 @@
         <v>66</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E9" s="32">
         <v>0</v>
@@ -22623,13 +23198,13 @@
         <v>180</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C10" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E10" s="44">
         <f>119.417644969154</f>
@@ -22644,13 +23219,13 @@
         <v>185</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C11" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E11" s="44">
         <f t="shared" ref="E11:E12" si="0">119.417644969154</f>
@@ -22671,7 +23246,7 @@
         <v>66</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E12" s="32">
         <f t="shared" si="0"/>
@@ -22692,7 +23267,7 @@
         <v>66</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E13" s="32">
         <v>0</v>
@@ -22710,7 +23285,7 @@
         <v>66</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E14" s="32">
         <v>0</v>
@@ -22728,7 +23303,7 @@
         <v>66</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E15" s="32">
         <v>0</v>
@@ -22746,7 +23321,7 @@
         <v>66</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E16" s="32">
         <v>-171.73</v>
@@ -22766,7 +23341,7 @@
         <v>66</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E17" s="32">
         <v>-171.73</v>
@@ -22786,7 +23361,7 @@
         <v>66</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E18" s="32">
         <v>0</v>
@@ -22804,7 +23379,7 @@
         <v>66</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E19" s="32">
         <f>202.32*0.05</f>
@@ -22825,7 +23400,7 @@
         <v>66</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E20" s="32">
         <f>202.32*0.95</f>
@@ -22846,7 +23421,7 @@
         <v>66</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E21" s="32">
         <f>202.32*0.01</f>
@@ -22867,7 +23442,7 @@
         <v>66</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E22" s="32">
         <f>202.32*0.99</f>
@@ -22882,13 +23457,13 @@
         <v>167</v>
       </c>
       <c r="B23" s="44" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C23" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E23" s="44">
         <f>202.32</f>
@@ -22909,7 +23484,7 @@
         <v>66</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E24" s="32">
         <f>118.6*0.05</f>
@@ -22930,7 +23505,7 @@
         <v>66</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E25" s="32">
         <f>118.6*0.95</f>
@@ -22951,7 +23526,7 @@
         <v>66</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E26" s="32">
         <f>118.6*0.03</f>
@@ -22972,7 +23547,7 @@
         <v>66</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E27" s="32">
         <f>118.6*0.97</f>
@@ -22987,13 +23562,13 @@
         <v>183</v>
       </c>
       <c r="B28" s="44" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C28" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E28" s="44">
         <f>118.6</f>
@@ -23008,13 +23583,13 @@
         <v>184</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C29" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E29" s="44">
         <f>118.6</f>
@@ -23035,7 +23610,7 @@
         <v>66</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E30" s="32">
         <f>118.6*0.05</f>
@@ -23056,7 +23631,7 @@
         <v>66</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E31" s="32">
         <f>118.6*0.95</f>
@@ -23077,7 +23652,7 @@
         <v>66</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E32" s="32">
         <f>118.6*0.03</f>
@@ -23098,7 +23673,7 @@
         <v>66</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E33" s="32">
         <f>118.6*0.97</f>
@@ -23113,13 +23688,13 @@
         <v>188</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C34" s="44" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E34" s="44">
         <f>118.6</f>
@@ -23140,7 +23715,7 @@
         <v>153</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E35" s="32">
         <v>-1</v>
@@ -23160,13 +23735,13 @@
         <v>153</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E36" s="32">
         <v>-1</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75">
@@ -23180,455 +23755,476 @@
         <v>153</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E37" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="12.75">
-      <c r="A38" s="4" t="s">
-        <v>298</v>
+    <row r="38" spans="1:6" s="22" customFormat="1" ht="12.75">
+      <c r="A38" s="46" t="s">
+        <v>344</v>
       </c>
       <c r="B38" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C38" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="D38" s="32" t="s">
+      <c r="C38" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="E38" s="32">
-        <v>0</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>302</v>
+      <c r="D38" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" s="46">
+        <v>1</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="22" customFormat="1" ht="12.75">
       <c r="A39" s="46" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B39" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D39" s="44" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E39" s="46">
         <v>1</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="22" customFormat="1" ht="12.75">
       <c r="A40" s="46" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="B40" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C40" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D40" s="44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E40" s="46">
         <v>1</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="22" customFormat="1" ht="12.75">
       <c r="A41" s="46" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B41" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D41" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E41" s="46">
         <v>1</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="22" customFormat="1" ht="12.75">
       <c r="A42" s="46" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B42" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E42" s="46">
         <v>1</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="22" customFormat="1" ht="12.75">
       <c r="A43" s="46" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="B43" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="E43" s="46">
         <v>1</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="22" customFormat="1" ht="12.75">
       <c r="A44" s="46" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B44" s="32" t="s">
         <v>141</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D44" s="44" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E44" s="46">
         <v>1</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="22" customFormat="1" ht="12.75">
-      <c r="A45" s="46" t="s">
-        <v>338</v>
-      </c>
-      <c r="B45" s="32" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="50" customFormat="1" ht="12.75">
+      <c r="A45" s="49" t="s">
+        <v>347</v>
+      </c>
+      <c r="B45" s="49" t="s">
         <v>141</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D45" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="E45" s="46">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="E45" s="49">
+        <v>0.05</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="50" customFormat="1" ht="12.75">
       <c r="A46" s="49" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B46" s="49" t="s">
         <v>141</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D46" s="44" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E46" s="49">
         <v>0.05</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="50" customFormat="1" ht="12.75">
       <c r="A47" s="49" t="s">
-        <v>351</v>
+        <v>311</v>
       </c>
       <c r="B47" s="49" t="s">
         <v>141</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D47" s="44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E47" s="49">
         <v>0.05</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="50" customFormat="1" ht="12.75">
       <c r="A48" s="49" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B48" s="49" t="s">
         <v>141</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D48" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E48" s="49">
         <v>0.05</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="50" customFormat="1" ht="12.75">
       <c r="A49" s="49" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B49" s="49" t="s">
         <v>141</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D49" s="44" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E49" s="49">
         <v>0.05</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="50" customFormat="1" ht="12.75">
       <c r="A50" s="49" t="s">
-        <v>316</v>
+        <v>349</v>
       </c>
       <c r="B50" s="49" t="s">
         <v>141</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D50" s="44" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="E50" s="49">
         <v>0.05</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="50" customFormat="1" ht="12.75">
       <c r="A51" s="49" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="B51" s="49" t="s">
         <v>141</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D51" s="44" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E51" s="49">
         <v>0.05</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="50" customFormat="1" ht="12.75">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="48" customFormat="1" ht="12.75">
       <c r="A52" s="49" t="s">
-        <v>317</v>
-      </c>
-      <c r="B52" s="49" t="s">
-        <v>141</v>
+        <v>347</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>140</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D52" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="E52" s="49">
-        <v>0.05</v>
+        <v>180</v>
+      </c>
+      <c r="E52" s="47">
+        <v>0.95</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="48" customFormat="1" ht="12.75">
       <c r="A53" s="49" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B53" s="47" t="s">
         <v>140</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D53" s="44" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E53" s="47">
         <v>0.95</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="48" customFormat="1" ht="12.75">
       <c r="A54" s="49" t="s">
-        <v>351</v>
+        <v>311</v>
       </c>
       <c r="B54" s="47" t="s">
         <v>140</v>
       </c>
       <c r="C54" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E54" s="47">
         <v>0.95</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="48" customFormat="1" ht="12.75">
       <c r="A55" s="49" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B55" s="47" t="s">
         <v>140</v>
       </c>
       <c r="C55" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D55" s="44" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E55" s="47">
         <v>0.95</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="48" customFormat="1" ht="12.75">
       <c r="A56" s="49" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B56" s="47" t="s">
         <v>140</v>
       </c>
       <c r="C56" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E56" s="47">
         <v>0.95</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="48" customFormat="1" ht="12.75">
       <c r="A57" s="49" t="s">
-        <v>316</v>
+        <v>349</v>
       </c>
       <c r="B57" s="47" t="s">
         <v>140</v>
       </c>
       <c r="C57" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D57" s="44" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="E57" s="47">
         <v>0.95</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="48" customFormat="1" ht="12.75">
       <c r="A58" s="49" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="B58" s="47" t="s">
         <v>140</v>
       </c>
       <c r="C58" s="44" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E58" s="47">
         <v>0.95</v>
       </c>
       <c r="F58" s="23" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="48" customFormat="1" ht="12.75">
-      <c r="A59" s="49" t="s">
-        <v>317</v>
-      </c>
-      <c r="B59" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="C59" s="44" t="s">
-        <v>346</v>
-      </c>
-      <c r="D59" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="E59" s="47">
-        <v>0.95</v>
-      </c>
-      <c r="F59" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="12.75">
+      <c r="A59" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="E59" s="32">
+        <v>0</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="12.75">
+      <c r="A60" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="E60" s="32">
+        <v>0</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -51676,7 +52272,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -52101,16 +52697,16 @@
         <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>296</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G2" s="28">
         <v>0.154</v>
@@ -52214,16 +52810,16 @@
         <v>38</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>296</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G3" s="28">
         <v>0.153</v>
@@ -52327,16 +52923,16 @@
         <v>39</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>296</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G4" s="28">
         <v>0.152</v>
@@ -52440,16 +53036,16 @@
         <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>295</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G5" s="26">
         <v>0.15</v>
@@ -52553,16 +53149,16 @@
         <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>295</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G6" s="26">
         <v>0.15</v>
@@ -52666,16 +53262,16 @@
         <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>295</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G7" s="26">
         <v>0.15</v>
@@ -52779,16 +53375,16 @@
         <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>198</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G8" s="26">
         <v>0.24</v>
@@ -52892,16 +53488,16 @@
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>198</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G9" s="26">
         <v>0.23</v>
@@ -53005,16 +53601,16 @@
         <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>198</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G10" s="26">
         <v>0.23</v>
@@ -53124,10 +53720,10 @@
         <v>195</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G11" s="4">
         <v>0.215</v>
@@ -55891,7 +56487,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="46" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>19</v>
@@ -55911,7 +56507,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="46" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>19</v>
@@ -55931,7 +56527,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="46" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>19</v>
@@ -55951,7 +56547,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="46" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>19</v>
@@ -55971,7 +56567,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="46" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>19</v>
@@ -55991,7 +56587,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="46" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>16</v>
@@ -56011,7 +56607,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="46" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>16</v>
@@ -56031,7 +56627,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="49" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>19</v>
@@ -56051,7 +56647,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="49" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>19</v>
@@ -56071,7 +56667,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="49" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>19</v>
@@ -56091,7 +56687,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="49" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>19</v>
@@ -56111,7 +56707,7 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="49" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>19</v>
@@ -56131,7 +56727,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="49" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>16</v>
@@ -56151,7 +56747,7 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="49" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>16</v>

</xml_diff>